<commit_message>
Implemented the Multiply Tests
</commit_message>
<xml_diff>
--- a/BongzAutomationLabz/src/test/resources/excel/Book1.xlsx
+++ b/BongzAutomationLabz/src/test/resources/excel/Book1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="204" windowWidth="15300" windowHeight="4188" activeTab="1"/>
+    <workbookView xWindow="384" yWindow="204" windowWidth="15300" windowHeight="4188"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="31">
   <si>
     <t>testname</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>sdgdf</t>
+  </si>
+  <si>
+    <t>multiplyRewardsTest</t>
+  </si>
+  <si>
+    <t>To check multiply rewards test</t>
   </si>
 </sst>
 </file>
@@ -444,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,7 +519,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
@@ -524,13 +530,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
@@ -541,10 +547,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -563,10 +569,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,7 +689,7 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -700,7 +706,7 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
@@ -726,6 +732,23 @@
         <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented docker in the framework
</commit_message>
<xml_diff>
--- a/BongzAutomationLabz/src/test/resources/excel/Book1.xlsx
+++ b/BongzAutomationLabz/src/test/resources/excel/Book1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="204" windowWidth="15300" windowHeight="4188"/>
+    <workbookView xWindow="384" yWindow="204" windowWidth="15300" windowHeight="4188" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="33">
   <si>
     <t>testname</t>
   </si>
@@ -87,9 +87,6 @@
     <t>bomaseko1</t>
   </si>
   <si>
-    <t>@KBTokzan4078</t>
-  </si>
-  <si>
     <t>multiplyLoginLogoutTest</t>
   </si>
   <si>
@@ -109,6 +106,15 @@
   </si>
   <si>
     <t>To check multiply rewards test</t>
+  </si>
+  <si>
+    <t>@KBTokzan2021</t>
+  </si>
+  <si>
+    <t>multiplyOptionsTest</t>
+  </si>
+  <si>
+    <t>To check multiply options test</t>
   </si>
 </sst>
 </file>
@@ -448,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,13 +519,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
@@ -530,10 +536,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
         <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -547,11 +553,11 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
         <v>29</v>
       </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
@@ -559,6 +565,23 @@
         <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -569,10 +592,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,7 +692,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -686,7 +709,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -698,12 +721,12 @@
         <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -712,15 +735,15 @@
         <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
@@ -729,15 +752,15 @@
         <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -746,10 +769,27 @@
         <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented the browser version
</commit_message>
<xml_diff>
--- a/BongzAutomationLabz/src/test/resources/excel/Book1.xlsx
+++ b/BongzAutomationLabz/src/test/resources/excel/Book1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="37">
   <si>
     <t>testname</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t>To check multiply options test</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>79.0.3945.117</t>
+  </si>
+  <si>
+    <t>88.0.4324.96</t>
+  </si>
+  <si>
+    <t>85.0</t>
   </si>
 </sst>
 </file>
@@ -457,7 +469,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,7 +537,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
@@ -576,7 +588,7 @@
         <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
@@ -592,20 +604,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -616,13 +628,16 @@
         <v>18</v>
       </c>
       <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -632,14 +647,17 @@
       <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -649,14 +667,17 @@
       <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -666,14 +687,17 @@
       <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -683,31 +707,37 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -717,14 +747,17 @@
       <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -735,13 +768,16 @@
         <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -752,13 +788,16 @@
         <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -769,13 +808,16 @@
         <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -786,14 +828,18 @@
         <v>19</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="F11" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>